<commit_message>
#2082 Updated Secondary Auditors Workbook For Cypress Tests
</commit_message>
<xml_diff>
--- a/backend/cypress/fixtures/test_workbooks/secondary-auditors-workbook.xlsx
+++ b/backend/cypress/fixtures/test_workbooks/secondary-auditors-workbook.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hd\Desktop\GSA\FAC\backend\cypress\fixtures\test_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C97173-0CE5-4FF6-88B9-C21F90258F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB650E2F-CB1A-4D66-AFE1-7D8A2712CC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="32580" yWindow="2985" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32850" yWindow="2550" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coversheet" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Federal Audit Clearinghouse
 fac.gov</t>
@@ -284,25 +284,31 @@
     <t>D7A4J33FUMJ1</t>
   </si>
   <si>
-    <t>Very Amazing Auditing Firm</t>
+    <t xml:space="preserve">Very Amazing </t>
   </si>
   <si>
-    <t>ABCDEFGHI</t>
+    <t>123456789</t>
   </si>
   <si>
     <t>7832 Richmond Hwy Hybla Valley</t>
   </si>
   <si>
+    <t>Alexandria</t>
+  </si>
+  <si>
+    <t>22306</t>
+  </si>
+  <si>
+    <t>Auditor</t>
+  </si>
+  <si>
     <t>John Smith</t>
   </si>
   <si>
-    <t>Auditor (Title)</t>
+    <t>test@a.gov</t>
   </si>
   <si>
-    <t>a@a.gov</t>
-  </si>
-  <si>
-    <t>Alexandria</t>
+    <t>555-555-5555</t>
   </si>
 </sst>
 </file>
@@ -678,7 +684,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,25 +797,25 @@
         <v>78</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="4">
-        <v>22306</v>
+      <c r="F2" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
-      <c r="I2" s="4">
-        <v>5555555555</v>
+      <c r="I2" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>